<commit_message>
Update importing files from Robot Structural Analysis
</commit_message>
<xml_diff>
--- a/tests/test_data/filtered_results.xlsx
+++ b/tests/test_data/filtered_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>member</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>compression perpendicular (dcr)</t>
+  </si>
+  <si>
+    <t>elemento 1</t>
+  </si>
+  <si>
+    <t>sección 1</t>
+  </si>
+  <si>
+    <t>sección 2</t>
+  </si>
+  <si>
+    <t>force_3</t>
+  </si>
+  <si>
+    <t>force_4</t>
+  </si>
+  <si>
+    <t>force_2</t>
+  </si>
+  <si>
+    <t>force_1</t>
   </si>
 </sst>
 </file>
@@ -428,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,6 +514,478 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>0.5952380952380952</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0.02240896358543417</v>
+      </c>
+      <c r="M2">
+        <v>0.02240896358543417</v>
+      </c>
+      <c r="N2">
+        <v>0.5952380952380952</v>
+      </c>
+      <c r="O2">
+        <v>0.3767173536081099</v>
+      </c>
+      <c r="P2">
+        <v>0.004581901489117984</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>0.119047619047619</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+      <c r="G3">
+        <v>400</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="M3">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="N3">
+        <v>0.119047619047619</v>
+      </c>
+      <c r="O3">
+        <v>0.02649726557289582</v>
+      </c>
+      <c r="P3">
+        <v>0.004581901489117984</v>
+      </c>
+      <c r="Q3">
+        <v>0.009163802978235968</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>1.066098081023454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="M4">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.0123249299719888</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>0.004581901489117984</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0.5602240896358543</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0.5602240896358543</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0.004581901489117984</v>
+      </c>
+      <c r="Q5">
+        <v>0.004581901489117984</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>0.5330490405117271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0.002976190476190476</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>10000</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1.120448179271709E-05</v>
+      </c>
+      <c r="M6">
+        <v>1.120448179271709E-05</v>
+      </c>
+      <c r="N6">
+        <v>0.002976190476190476</v>
+      </c>
+      <c r="O6">
+        <v>2.006219154328398E-05</v>
+      </c>
+      <c r="P6">
+        <v>2.290950744558992E-05</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>0.0005952380952380953</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2000</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="M7">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="N7">
+        <v>0.0005952380952380953</v>
+      </c>
+      <c r="O7">
+        <v>5.676437241563292E-06</v>
+      </c>
+      <c r="P7">
+        <v>2.290950744558992E-05</v>
+      </c>
+      <c r="Q7">
+        <v>4.581901489117984E-05</v>
+      </c>
+      <c r="R7">
+        <v>20</v>
+      </c>
+      <c r="S7">
+        <v>1.066098081023454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>2.290950744558992E-05</v>
+      </c>
+      <c r="E8">
+        <v>10000</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>0.002801120448179272</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0.002801120448179272</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>2.290950744558992E-05</v>
+      </c>
+      <c r="Q8">
+        <v>2.290950744558992E-05</v>
+      </c>
+      <c r="R8">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <v>0.5330490405117271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>400</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="M9">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>5.322128851540616E-06</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Examples and readme finished
</commit_message>
<xml_diff>
--- a/tests/test_data/filtered_results.xlsx
+++ b/tests/test_data/filtered_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>member</t>
   </si>
@@ -67,22 +67,22 @@
     <t>bending and compression (dcr)</t>
   </si>
   <si>
+    <t>compression perpendicular</t>
+  </si>
+  <si>
+    <t>compression perpendicular (dcr)</t>
+  </si>
+  <si>
     <t>elemento 1</t>
   </si>
   <si>
+    <t>elemento 2</t>
+  </si>
+  <si>
+    <t>elemento 3</t>
+  </si>
+  <si>
     <t>sección 1</t>
-  </si>
-  <si>
-    <t>sección 2</t>
-  </si>
-  <si>
-    <t>force_1</t>
-  </si>
-  <si>
-    <t>force_3</t>
-  </si>
-  <si>
-    <t>force_4</t>
   </si>
   <si>
     <t>force_2</t>
@@ -443,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,137 +501,155 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>0.5511463844797179</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>20000</v>
+      </c>
+      <c r="H2">
+        <v>0.5511463844797179</v>
+      </c>
+      <c r="I2">
+        <v>400</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>0.005708628981930893</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0.005708628981930893</v>
+      </c>
+      <c r="Q2">
+        <v>0.3094709661069959</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>0.5952380952380952</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>10000</v>
-      </c>
-      <c r="H2">
-        <v>0.5952380952380952</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>0.004581901489117984</v>
-      </c>
-      <c r="O2">
-        <v>0.004581901489117984</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0.3543083900226757</v>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>0.5511463844797179</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>20000</v>
+      </c>
+      <c r="H3">
+        <v>0.5511463844797179</v>
+      </c>
+      <c r="I3">
+        <v>400</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>0.005708628981930893</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.005708628981930893</v>
+      </c>
+      <c r="Q3">
+        <v>0.3094709661069959</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>0.02240896358543417</v>
-      </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-      <c r="F3">
-        <v>0.5602240896358543</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1000</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0.02240896358543417</v>
-      </c>
-      <c r="L3">
-        <v>10</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0.004581901489117984</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0.5826330532212886</v>
-      </c>
-      <c r="Q3">
-        <v>0.02240896358543417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4">
-        <v>0.0123249299719888</v>
+        <v>0.5511463844797179</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>20000</v>
       </c>
-      <c r="F4">
-        <v>1.120448179271709</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.5511463844797179</v>
       </c>
       <c r="I4">
         <v>400</v>
@@ -640,237 +658,31 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>0.0123249299719888</v>
+        <v>0.005708628981930893</v>
       </c>
       <c r="L4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0.004581901489117984</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>0.009163802978235968</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1.132773109243697</v>
+        <v>0.005708628981930893</v>
       </c>
       <c r="Q4">
-        <v>0.0123249299719888</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <v>0.005952380952380952</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>20000</v>
-      </c>
-      <c r="H5">
-        <v>0.005952380952380952</v>
-      </c>
-      <c r="I5">
-        <v>400</v>
-      </c>
-      <c r="J5">
-        <v>50</v>
-      </c>
-      <c r="K5">
-        <v>5.322128851540616E-06</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>5.322128851540616E-06</v>
-      </c>
-      <c r="Q5">
-        <v>4.075296785380818E-05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>0.002976190476190476</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>10000</v>
-      </c>
-      <c r="H6">
-        <v>0.002976190476190476</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <v>10</v>
-      </c>
-      <c r="N6">
-        <v>2.290950744558992E-05</v>
-      </c>
-      <c r="O6">
-        <v>2.290950744558992E-05</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>8.857709750566892E-06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7">
-        <v>4.581901489117984E-05</v>
-      </c>
-      <c r="E7">
-        <v>20000</v>
-      </c>
-      <c r="F7">
-        <v>0.005602240896358543</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>400</v>
-      </c>
-      <c r="J7">
-        <v>50</v>
-      </c>
-      <c r="K7">
-        <v>5.322128851540616E-06</v>
-      </c>
-      <c r="L7">
-        <v>10</v>
-      </c>
-      <c r="M7">
-        <v>20</v>
-      </c>
-      <c r="N7">
-        <v>2.290950744558992E-05</v>
-      </c>
-      <c r="O7">
-        <v>4.581901489117984E-05</v>
-      </c>
-      <c r="P7">
-        <v>0.005607563025210084</v>
-      </c>
-      <c r="Q7">
-        <v>5.322128851540616E-06</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8">
-        <v>2.290950744558992E-05</v>
-      </c>
-      <c r="E8">
-        <v>10000</v>
-      </c>
-      <c r="F8">
-        <v>0.002801120448179272</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1000</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>1.120448179271709E-05</v>
-      </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>2.290950744558992E-05</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0.002812324929971989</v>
-      </c>
-      <c r="Q8">
-        <v>1.120448179271709E-05</v>
+        <v>0.3094709661069959</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>